<commit_message>
testato tutto e funzionante - manca da sistemare la numerazione del template MVskid
</commit_message>
<xml_diff>
--- a/template_excel/template_EH05HD_PEMS_TCCexp.xlsx
+++ b/template_excel/template_EH05HD_PEMS_TCCexp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhoaenergy.sharepoint.com/sites/Q1043-HyESScontainerHDevolution/Documenti condivisi/General/08_SW standardization/11_Alarms_Template/Alarms_automation_EH+PH/template_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="279" documentId="13_ncr:1_{0E8DEEBE-11A6-45AE-A2F5-9C72511D066D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{878877E5-CF08-4A1F-A1DE-ED991B913F0B}"/>
+  <xr:revisionPtr revIDLastSave="313" documentId="13_ncr:1_{0E8DEEBE-11A6-45AE-A2F5-9C72511D066D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{585FBB21-37D2-4200-960A-03219838B6E2}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,36 +311,6 @@
     <t>A | Socomec Modbus communication error | PEMS</t>
   </si>
   <si>
-    <t>A | HVAC2_5 Modbus RTU communication error | PEMS</t>
-  </si>
-  <si>
-    <t>A | HVAC2_4 Modbus RTU communication error | PEMS</t>
-  </si>
-  <si>
-    <t>A | HVAC2_3 Modbus RTU communication error | PEMS</t>
-  </si>
-  <si>
-    <t>A | HVAC2_2 Modbus RTU communication error | PEMS</t>
-  </si>
-  <si>
-    <t>A | HVAC2_1 Modbus RTU communication error | PEMS</t>
-  </si>
-  <si>
-    <t>A | HVAC1_5 Modbus RTU communication error | PEMS</t>
-  </si>
-  <si>
-    <t>A | HVAC1_4 Modbus RTU communication error | PEMS</t>
-  </si>
-  <si>
-    <t>A | HVAC1_3 Modbus RTU communication error | PEMS</t>
-  </si>
-  <si>
-    <t>A | HVAC1_2 Modbus RTU communication error | PEMS</t>
-  </si>
-  <si>
-    <t>A | HVAC1_1 Modbus RTU communication error | PEMS</t>
-  </si>
-  <si>
     <t>A | Battery room high single temperature | PEMS</t>
   </si>
   <si>
@@ -432,36 +402,6 @@
   </si>
   <si>
     <t>W | Spare wHMI_Warning2.15 | PEMS</t>
-  </si>
-  <si>
-    <t>W | Spare wHMI_Warning3.2 | PEMS</t>
-  </si>
-  <si>
-    <t>W | Spare wHMI_Warning3.3 | PEMS</t>
-  </si>
-  <si>
-    <t>W | Spare wHMI_Warning3.4 | PEMS</t>
-  </si>
-  <si>
-    <t>W | Spare wHMI_Warning3.5 | PEMS</t>
-  </si>
-  <si>
-    <t>W | Spare wHMI_Warning3.6 | PEMS</t>
-  </si>
-  <si>
-    <t>W | Spare wHMI_Warning3.7 | PEMS</t>
-  </si>
-  <si>
-    <t>W | Spare wHMI_Warning3.8 | PEMS</t>
-  </si>
-  <si>
-    <t>W | Spare wHMI_Warning3.9 | PEMS</t>
-  </si>
-  <si>
-    <t>W | Spare wHMI_Warning3.10 | PEMS</t>
-  </si>
-  <si>
-    <t>W | Spare wHMI_Warning3.11 | PEMS</t>
   </si>
   <si>
     <t>W | Spare wHMI_Warning3.12 | PEMS</t>
@@ -566,12 +506,6 @@
     <t>W |  HVAC General Alarm | HVAC5, BB2</t>
   </si>
   <si>
-    <t>A | Door opened PEMS | 537S5,PEMS</t>
-  </si>
-  <si>
-    <t>A | Door opened PWC | 537S6,PEMS</t>
-  </si>
-  <si>
     <t>A | Door opened HVAC 2_5 | 537S4,PEMS</t>
   </si>
   <si>
@@ -612,6 +546,72 @@
   </si>
   <si>
     <t>A | Disconnector open | PWC001-A,PEMS</t>
+  </si>
+  <si>
+    <t>A | Spare wHMI_Alarm4.4 | PEMS</t>
+  </si>
+  <si>
+    <t>A | Spare wHMI_Alarm4.6 | PEMS</t>
+  </si>
+  <si>
+    <t>A | Spare wHMI_Alarm4.5 | PEMS</t>
+  </si>
+  <si>
+    <t>A | Spare wHMI_Alarm4.7 | PEMS</t>
+  </si>
+  <si>
+    <t>A | Spare wHMI_Alarm4.8 | PEMS</t>
+  </si>
+  <si>
+    <t>A | Spare wHMI_Alarm4.9 | PEMS</t>
+  </si>
+  <si>
+    <t>A | Spare wHMI_Alarm4.0 | PEMS</t>
+  </si>
+  <si>
+    <t>A | Spare wHMI_Alarm4.1 | PEMS</t>
+  </si>
+  <si>
+    <t>A | Spare wHMI_Alarm4.2 | PEMS</t>
+  </si>
+  <si>
+    <t>A | Spare wHMI_Alarm4.3 | PEMS</t>
+  </si>
+  <si>
+    <t>W | Door opened PEMS | 537S5,PEMS</t>
+  </si>
+  <si>
+    <t>W | Door opened PWC | 537S6,PEMS</t>
+  </si>
+  <si>
+    <t>W | HVAC1_1 Modbus RTU communication error | PEMS</t>
+  </si>
+  <si>
+    <t>W | HVAC1_2 Modbus RTU communication error | PEMS</t>
+  </si>
+  <si>
+    <t>W | HVAC1_3 Modbus RTU communication error | PEMS</t>
+  </si>
+  <si>
+    <t>W | HVAC1_4 Modbus RTU communication error | PEMS</t>
+  </si>
+  <si>
+    <t>W | HVAC1_5 Modbus RTU communication error | PEMS</t>
+  </si>
+  <si>
+    <t>W | HVAC2_1 Modbus RTU communication error | PEMS</t>
+  </si>
+  <si>
+    <t>W | HVAC2_2 Modbus RTU communication error | PEMS</t>
+  </si>
+  <si>
+    <t>W | HVAC2_3 Modbus RTU communication error | PEMS</t>
+  </si>
+  <si>
+    <t>W | HVAC2_4 Modbus RTU communication error | PEMS</t>
+  </si>
+  <si>
+    <t>W | HVAC2_5 Modbus RTU communication error | PEMS</t>
   </si>
 </sst>
 </file>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1852,7 +1852,7 @@
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -2674,7 +2674,7 @@
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -3085,7 +3085,7 @@
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -3222,7 +3222,7 @@
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
@@ -3359,7 +3359,7 @@
     </row>
     <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
@@ -3496,7 +3496,7 @@
     </row>
     <row r="19" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
@@ -3633,7 +3633,7 @@
     </row>
     <row r="20" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -3770,7 +3770,7 @@
     </row>
     <row r="21" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -3907,7 +3907,7 @@
     </row>
     <row r="22" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="23" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
@@ -4181,7 +4181,7 @@
     </row>
     <row r="24" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
@@ -4318,7 +4318,7 @@
     </row>
     <row r="25" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="26" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -4592,7 +4592,7 @@
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
@@ -4729,7 +4729,7 @@
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -4866,7 +4866,7 @@
     </row>
     <row r="29" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
@@ -5003,7 +5003,7 @@
     </row>
     <row r="30" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
@@ -5140,7 +5140,7 @@
     </row>
     <row r="31" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
@@ -5277,7 +5277,7 @@
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
@@ -7195,7 +7195,7 @@
     </row>
     <row r="46" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
@@ -7332,7 +7332,7 @@
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="B47" t="s">
         <v>1</v>
@@ -8428,7 +8428,7 @@
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B55" t="s">
         <v>1</v>
@@ -8565,7 +8565,7 @@
     </row>
     <row r="56" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B56" t="s">
         <v>1</v>
@@ -8702,7 +8702,7 @@
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B57" t="s">
         <v>1</v>
@@ -8839,7 +8839,7 @@
     </row>
     <row r="58" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B58" t="s">
         <v>1</v>
@@ -8976,7 +8976,7 @@
     </row>
     <row r="59" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B59" t="s">
         <v>1</v>
@@ -9113,7 +9113,7 @@
     </row>
     <row r="60" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="B60" t="s">
         <v>1</v>
@@ -9250,7 +9250,7 @@
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="B61" t="s">
         <v>1</v>
@@ -9387,7 +9387,7 @@
     </row>
     <row r="62" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
@@ -9524,7 +9524,7 @@
     </row>
     <row r="63" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="B63" t="s">
         <v>1</v>
@@ -9661,7 +9661,7 @@
     </row>
     <row r="64" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="B64" t="s">
         <v>1</v>
@@ -9798,7 +9798,7 @@
     </row>
     <row r="65" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="B65" t="s">
         <v>1</v>
@@ -9935,7 +9935,7 @@
     </row>
     <row r="66" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="B66" t="s">
         <v>1</v>
@@ -10072,7 +10072,7 @@
     </row>
     <row r="67" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="B67" t="s">
         <v>1</v>
@@ -10209,7 +10209,7 @@
     </row>
     <row r="68" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="B68" t="s">
         <v>1</v>
@@ -10346,7 +10346,7 @@
     </row>
     <row r="69" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="B69" t="s">
         <v>1</v>
@@ -10483,7 +10483,7 @@
     </row>
     <row r="70" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="B70" t="s">
         <v>1</v>
@@ -10620,7 +10620,7 @@
     </row>
     <row r="71" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="B71" t="s">
         <v>1</v>
@@ -10757,7 +10757,7 @@
     </row>
     <row r="72" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="B72" t="s">
         <v>1</v>
@@ -10894,7 +10894,7 @@
     </row>
     <row r="73" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="B73" t="s">
         <v>1</v>
@@ -11031,7 +11031,7 @@
     </row>
     <row r="74" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
@@ -11168,7 +11168,7 @@
     </row>
     <row r="75" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B75" t="s">
         <v>1</v>
@@ -11305,7 +11305,7 @@
     </row>
     <row r="76" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B76" t="s">
         <v>1</v>
@@ -11442,7 +11442,7 @@
     </row>
     <row r="77" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
@@ -11579,7 +11579,7 @@
     </row>
     <row r="78" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B78" t="s">
         <v>1</v>
@@ -11716,7 +11716,7 @@
     </row>
     <row r="79" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
@@ -11853,7 +11853,7 @@
     </row>
     <row r="80" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
@@ -11989,8 +11989,8 @@
       </c>
     </row>
     <row r="81" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>101</v>
+      <c r="A81" t="s">
+        <v>177</v>
       </c>
       <c r="B81" t="s">
         <v>1</v>
@@ -12126,8 +12126,8 @@
       </c>
     </row>
     <row r="82" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
-        <v>100</v>
+      <c r="A82" t="s">
+        <v>178</v>
       </c>
       <c r="B82" t="s">
         <v>1</v>
@@ -12263,8 +12263,8 @@
       </c>
     </row>
     <row r="83" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>99</v>
+      <c r="A83" t="s">
+        <v>179</v>
       </c>
       <c r="B83" t="s">
         <v>1</v>
@@ -12400,8 +12400,8 @@
       </c>
     </row>
     <row r="84" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
-        <v>98</v>
+      <c r="A84" t="s">
+        <v>180</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
@@ -12537,8 +12537,8 @@
       </c>
     </row>
     <row r="85" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
-        <v>97</v>
+      <c r="A85" t="s">
+        <v>171</v>
       </c>
       <c r="B85" t="s">
         <v>1</v>
@@ -12674,8 +12674,8 @@
       </c>
     </row>
     <row r="86" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>96</v>
+      <c r="A86" t="s">
+        <v>173</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
@@ -12811,8 +12811,8 @@
       </c>
     </row>
     <row r="87" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>95</v>
+      <c r="A87" t="s">
+        <v>172</v>
       </c>
       <c r="B87" t="s">
         <v>1</v>
@@ -12948,8 +12948,8 @@
       </c>
     </row>
     <row r="88" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
-        <v>94</v>
+      <c r="A88" t="s">
+        <v>174</v>
       </c>
       <c r="B88" t="s">
         <v>1</v>
@@ -13085,8 +13085,8 @@
       </c>
     </row>
     <row r="89" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>93</v>
+      <c r="A89" t="s">
+        <v>175</v>
       </c>
       <c r="B89" t="s">
         <v>1</v>
@@ -13222,8 +13222,8 @@
       </c>
     </row>
     <row r="90" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>92</v>
+      <c r="A90" t="s">
+        <v>176</v>
       </c>
       <c r="B90" t="s">
         <v>1</v>
@@ -13360,7 +13360,7 @@
     </row>
     <row r="91" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B91" t="s">
         <v>1</v>
@@ -13497,7 +13497,7 @@
     </row>
     <row r="92" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B92" t="s">
         <v>1</v>
@@ -13634,7 +13634,7 @@
     </row>
     <row r="93" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B93" t="s">
         <v>1</v>
@@ -15826,7 +15826,7 @@
     </row>
     <row r="109" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B109" t="s">
         <v>0</v>
@@ -15963,7 +15963,7 @@
     </row>
     <row r="110" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B110" t="s">
         <v>0</v>
@@ -16100,7 +16100,7 @@
     </row>
     <row r="111" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B111" t="s">
         <v>0</v>
@@ -16237,7 +16237,7 @@
     </row>
     <row r="112" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B112" t="s">
         <v>0</v>
@@ -16374,7 +16374,7 @@
     </row>
     <row r="113" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="B113" t="s">
         <v>0</v>
@@ -16511,7 +16511,7 @@
     </row>
     <row r="114" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="B114" t="s">
         <v>0</v>
@@ -16648,7 +16648,7 @@
     </row>
     <row r="115" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="B115" t="s">
         <v>0</v>
@@ -16785,7 +16785,7 @@
     </row>
     <row r="116" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="B116" t="s">
         <v>0</v>
@@ -16922,7 +16922,7 @@
     </row>
     <row r="117" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="B117" t="s">
         <v>0</v>
@@ -17059,7 +17059,7 @@
     </row>
     <row r="118" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="B118" t="s">
         <v>0</v>
@@ -17196,7 +17196,7 @@
     </row>
     <row r="119" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="B119" t="s">
         <v>0</v>
@@ -17333,7 +17333,7 @@
     </row>
     <row r="120" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="B120" t="s">
         <v>0</v>
@@ -17470,7 +17470,7 @@
     </row>
     <row r="121" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="B121" t="s">
         <v>0</v>
@@ -17607,7 +17607,7 @@
     </row>
     <row r="122" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="B122" t="s">
         <v>0</v>
@@ -17744,7 +17744,7 @@
     </row>
     <row r="123" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B123" t="s">
         <v>0</v>
@@ -17881,7 +17881,7 @@
     </row>
     <row r="124" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B124" t="s">
         <v>0</v>
@@ -18018,7 +18018,7 @@
     </row>
     <row r="125" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B125" t="s">
         <v>0</v>
@@ -18155,7 +18155,7 @@
     </row>
     <row r="126" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B126" t="s">
         <v>0</v>
@@ -18292,7 +18292,7 @@
     </row>
     <row r="127" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B127" t="s">
         <v>0</v>
@@ -18429,7 +18429,7 @@
     </row>
     <row r="128" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B128" t="s">
         <v>0</v>
@@ -18566,7 +18566,7 @@
     </row>
     <row r="129" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B129" t="s">
         <v>0</v>
@@ -18703,7 +18703,7 @@
     </row>
     <row r="130" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B130" t="s">
         <v>0</v>
@@ -18839,8 +18839,8 @@
       </c>
     </row>
     <row r="131" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>133</v>
+      <c r="A131" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="B131" t="s">
         <v>0</v>
@@ -18976,8 +18976,8 @@
       </c>
     </row>
     <row r="132" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>134</v>
+      <c r="A132" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="B132" t="s">
         <v>0</v>
@@ -19113,8 +19113,8 @@
       </c>
     </row>
     <row r="133" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>135</v>
+      <c r="A133" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="B133" t="s">
         <v>0</v>
@@ -19250,8 +19250,8 @@
       </c>
     </row>
     <row r="134" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>136</v>
+      <c r="A134" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B134" t="s">
         <v>0</v>
@@ -19387,8 +19387,8 @@
       </c>
     </row>
     <row r="135" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>137</v>
+      <c r="A135" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="B135" t="s">
         <v>0</v>
@@ -19524,8 +19524,8 @@
       </c>
     </row>
     <row r="136" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>138</v>
+      <c r="A136" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B136" t="s">
         <v>0</v>
@@ -19661,8 +19661,8 @@
       </c>
     </row>
     <row r="137" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>139</v>
+      <c r="A137" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="B137" t="s">
         <v>0</v>
@@ -19798,8 +19798,8 @@
       </c>
     </row>
     <row r="138" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
-        <v>140</v>
+      <c r="A138" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="B138" t="s">
         <v>0</v>
@@ -19935,8 +19935,8 @@
       </c>
     </row>
     <row r="139" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>141</v>
+      <c r="A139" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="B139" t="s">
         <v>0</v>
@@ -20072,8 +20072,8 @@
       </c>
     </row>
     <row r="140" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>142</v>
+      <c r="A140" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="B140" t="s">
         <v>0</v>
@@ -20210,7 +20210,7 @@
     </row>
     <row r="141" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B141" t="s">
         <v>0</v>
@@ -20347,7 +20347,7 @@
     </row>
     <row r="142" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="B142" t="s">
         <v>0</v>
@@ -20484,7 +20484,7 @@
     </row>
     <row r="143" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B143" t="s">
         <v>0</v>
@@ -20621,7 +20621,7 @@
     </row>
     <row r="144" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B144" t="s">
         <v>0</v>
@@ -22813,7 +22813,7 @@
     </row>
     <row r="160" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B160" t="s">
         <v>0</v>
@@ -25005,7 +25005,7 @@
     </row>
     <row r="176" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="B176" t="s">
         <v>0</v>
@@ -25153,6 +25153,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="013edbdd-9b27-46fe-aec1-397647bd8b02" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <b1b820adfd3e4a078472514c1a5cb5ff xmlns="013edbdd-9b27-46fe-aec1-397647bd8b02" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100260B53F379FC324F8380158707F79306" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb8e72d88c5d94be5f5d36f4a7df34db">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="013edbdd-9b27-46fe-aec1-397647bd8b02" xmlns:ns3="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba157fbbfa56f81f5e8d108156af0e8f" ns2:_="" ns3:_="">
     <xsd:import namespace="013edbdd-9b27-46fe-aec1-397647bd8b02"/>
@@ -25401,28 +25422,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1438FDF-2946-46F1-B8C5-0D18F499F79D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="37c203c8-3597-4bdf-989b-97f19aa19824"/>
+    <ds:schemaRef ds:uri="c781fbf3-278a-457c-9b0e-349b594aca68"/>
+    <ds:schemaRef ds:uri="013edbdd-9b27-46fe-aec1-397647bd8b02"/>
+    <ds:schemaRef ds:uri="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="013edbdd-9b27-46fe-aec1-397647bd8b02" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <b1b820adfd3e4a078472514c1a5cb5ff xmlns="013edbdd-9b27-46fe-aec1-397647bd8b02" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FDFF20-B1A7-49F0-B0E9-C0032B0436CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCAA4EA0-2B77-4AD6-9356-794BD2B990F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25439,25 +25460,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FDFF20-B1A7-49F0-B0E9-C0032B0436CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1438FDF-2946-46F1-B8C5-0D18F499F79D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="37c203c8-3597-4bdf-989b-97f19aa19824"/>
-    <ds:schemaRef ds:uri="c781fbf3-278a-457c-9b0e-349b594aca68"/>
-    <ds:schemaRef ds:uri="013edbdd-9b27-46fe-aec1-397647bd8b02"/>
-    <ds:schemaRef ds:uri="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>